<commit_message>
Revised v0.3.5 schematic + images. Fixed  1resistor reference in BOM
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.3/BOMs/v0.3.5_bom.xlsx
+++ b/reference/hardware/v0.3/BOMs/v0.3.5_bom.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26920" windowHeight="16560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26920" windowHeight="16560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Full Kit" sheetId="1" r:id="rId1"/>
@@ -829,13 +829,13 @@
     <t>2.49KXBK-ND</t>
   </si>
   <si>
-    <t>R1,R3,R61</t>
-  </si>
-  <si>
     <t>497-5981-5-ND</t>
   </si>
   <si>
     <t>Slightly different part from Digikey as they no longer stock the original version</t>
+  </si>
+  <si>
+    <t>R1,R3,R59</t>
   </si>
 </sst>
 </file>
@@ -1964,8 +1964,8 @@
   </sheetPr>
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView topLeftCell="D12" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3057,7 +3057,7 @@
         <v>95</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K23" s="2" t="str">
         <f>VLOOKUP(I23,'[1]Component List'!$L:$N,3,FALSE)</f>
@@ -3071,7 +3071,7 @@
         <v>12.08</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O23" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3326,7 +3326,7 @@
         <v>2</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>134</v>
@@ -4070,8 +4070,8 @@
   </sheetPr>
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5061,7 +5061,7 @@
         <v>95</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L23" s="6">
         <v>1.51</v>
@@ -5071,7 +5071,7 @@
         <v>9.06</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O23" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5104,7 +5104,7 @@
     </row>
     <row r="25" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
-        <f>LEN(B25)-LEN(SUBSTITUTE(B25,",",""))+1</f>
+        <f t="shared" ref="A25:A32" si="5">LEN(B25)-LEN(SUBSTITUTE(B25,",",""))+1</f>
         <v>3</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -5137,7 +5137,7 @@
         <v>0.08</v>
       </c>
       <c r="M25" s="6">
-        <f t="shared" ref="M25:M32" si="5">L25*A25</f>
+        <f t="shared" ref="M25:M32" si="6">L25*A25</f>
         <v>0.24</v>
       </c>
       <c r="N25" s="4"/>
@@ -5152,7 +5152,7 @@
     </row>
     <row r="26" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
-        <f>LEN(B26)-LEN(SUBSTITUTE(B26,",",""))+1</f>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="B26" s="24" t="s">
@@ -5185,7 +5185,7 @@
         <v>0.06</v>
       </c>
       <c r="M26" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.54</v>
       </c>
       <c r="N26" s="4"/>
@@ -5194,13 +5194,13 @@
         <v>9,1.00KXBK-ND</v>
       </c>
       <c r="P26" t="str">
-        <f t="shared" ref="P26:P32" si="6">"Resistor - " &amp; A26&amp;"x "&amp;C26</f>
+        <f t="shared" ref="P26:P32" si="7">"Resistor - " &amp; A26&amp;"x "&amp;C26</f>
         <v>Resistor - 9x 1k</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20">
-        <f>LEN(B27)-LEN(SUBSTITUTE(B27,",",""))+1</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="B27" s="25" t="s">
@@ -5229,7 +5229,7 @@
         <v>0.22</v>
       </c>
       <c r="M27" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.88</v>
       </c>
       <c r="N27" s="13" t="s">
@@ -5240,13 +5240,13 @@
         <v>4,A105963CT-ND</v>
       </c>
       <c r="P27" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Resistor - 4x 680</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
-        <f>LEN(B28)-LEN(SUBSTITUTE(B28,",",""))+1</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="B28" s="4" t="s">
@@ -5279,7 +5279,7 @@
         <v>0.11</v>
       </c>
       <c r="M28" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.66</v>
       </c>
       <c r="N28" s="4"/>
@@ -5288,17 +5288,17 @@
         <v>6,RNF14FTD470RCT-ND</v>
       </c>
       <c r="P28" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Resistor - 6x 470</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20">
-        <f>LEN(B29)-LEN(SUBSTITUTE(B29,",",""))+1</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>134</v>
@@ -5337,13 +5337,13 @@
         <v>3,2.49KXBK-ND</v>
       </c>
       <c r="P29" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Resistor - 3x 0.1% 2.49k</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="20">
-        <f>LEN(B30)-LEN(SUBSTITUTE(B30,",",""))+1</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -5376,7 +5376,7 @@
         <v>0.46</v>
       </c>
       <c r="M30" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.46</v>
       </c>
       <c r="N30" s="4" t="s">
@@ -5387,13 +5387,13 @@
         <v>1,3.9KADCT-ND</v>
       </c>
       <c r="P30" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Resistor - 1x 0.1% 3.9k</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20">
-        <f>LEN(B31)-LEN(SUBSTITUTE(B31,",",""))+1</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="B31" s="24" t="s">
@@ -5426,7 +5426,7 @@
         <v>0.1</v>
       </c>
       <c r="M31" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="N31" s="4"/>
@@ -5435,13 +5435,13 @@
         <v>8,100KXBK-ND</v>
       </c>
       <c r="P31" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Resistor - 8x 100k</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20">
-        <f>LEN(B32)-LEN(SUBSTITUTE(B32,",",""))+1</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="B32" s="24" t="s">
@@ -5474,7 +5474,7 @@
         <v>0.27</v>
       </c>
       <c r="M32" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.54</v>
       </c>
       <c r="N32" s="4"/>
@@ -5483,7 +5483,7 @@
         <v>2,160YCT-ND</v>
       </c>
       <c r="P32" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Resistor - 2x 160</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Part number tweaks for v0.3.5 board
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.3/BOMs/v0.3.5_bom.xlsx
+++ b/reference/hardware/v0.3/BOMs/v0.3.5_bom.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="245">
   <si>
     <t>QTY</t>
   </si>
@@ -697,15 +697,6 @@
   </si>
   <si>
     <t>Required for Assembly</t>
-  </si>
-  <si>
-    <t>R39,R40,R54</t>
-  </si>
-  <si>
-    <t>R10,R13,R16,R19,R21,R23,R24,R29,R30,R50,R51,R57,R58</t>
-  </si>
-  <si>
-    <t>R9,R12,R15,R18,R26,R28,R33,R34</t>
   </si>
   <si>
     <t>R2,R4,R6,R8,R22,R41</t>
@@ -836,6 +827,18 @@
   </si>
   <si>
     <t>R1,R3,R59</t>
+  </si>
+  <si>
+    <t>R54</t>
+  </si>
+  <si>
+    <t>R10,R13,R16,R19,R21,R23,R24,R29,R30,R39,R40,R50,R51,R57,R58</t>
+  </si>
+  <si>
+    <t>R9,R12,R15,R18</t>
+  </si>
+  <si>
+    <t>R1,R3,R26,R28,R33,R34,R59</t>
   </si>
 </sst>
 </file>
@@ -1964,7 +1967,7 @@
   </sheetPr>
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -2014,7 +2017,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>8</v>
@@ -2029,7 +2032,7 @@
         <v>126</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="Q1" s="21" t="s">
         <v>132</v>
@@ -2194,13 +2197,13 @@
         <v>175</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="L5" s="27">
         <v>0.32</v>
@@ -2248,13 +2251,13 @@
         <v>175</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="L6" s="27">
         <v>0.98</v>
@@ -2585,13 +2588,13 @@
         <v>192</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
@@ -2601,13 +2604,13 @@
         <v>175</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="L13" s="27">
         <v>0.36</v>
@@ -2659,7 +2662,7 @@
         <v>106</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="L14" s="27">
         <v>0.47</v>
@@ -2858,12 +2861,12 @@
         <v>127</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>176</v>
@@ -2872,10 +2875,10 @@
         <v>1935161</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="L19" s="26">
         <v>0.38</v>
@@ -2920,13 +2923,13 @@
         <v>176</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>96</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="L20" s="27">
         <v>0.1</v>
@@ -2971,7 +2974,7 @@
         <v>176</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>109</v>
@@ -3057,7 +3060,7 @@
         <v>95</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="K23" s="2" t="str">
         <f>VLOOKUP(I23,'[1]Component List'!$L:$N,3,FALSE)</f>
@@ -3071,7 +3074,7 @@
         <v>12.08</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="O23" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3113,10 +3116,10 @@
     <row r="25" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <f>LEN(B25)-LEN(SUBSTITUTE(B25,",",""))+1</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>198</v>
+        <v>241</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>44</v>
@@ -3133,42 +3136,42 @@
         <v>175</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>178</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="L25" s="27">
         <v>0.08</v>
       </c>
       <c r="M25" s="27">
         <f t="shared" ref="M25:M32" si="6">L25*A25</f>
-        <v>0.24</v>
+        <v>0.08</v>
       </c>
       <c r="N25" s="4"/>
       <c r="O25" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>3,10KQBK-ND</v>
+        <v>1,10KQBK-ND</v>
       </c>
       <c r="P25" t="str">
         <f t="shared" si="4"/>
-        <v>603-MFR-25FBF52-10K|3</v>
+        <v>603-MFR-25FBF52-10K|1</v>
       </c>
       <c r="Q25" t="str">
         <f>"Resistor - " &amp; A25&amp;"x "&amp;C25</f>
-        <v>Resistor - 3x 10k</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>Resistor - 1x 10k</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
         <f>LEN(B26)-LEN(SUBSTITUTE(B26,",",""))+1</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>199</v>
+        <v>242</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>47</v>
@@ -3185,42 +3188,42 @@
         <v>175</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>50</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="L26" s="27">
         <v>0.06</v>
       </c>
       <c r="M26" s="27">
         <f t="shared" si="6"/>
-        <v>0.78</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="N26" s="4"/>
       <c r="O26" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>13,1.00KXBK-ND</v>
+        <v>15,1.00KXBK-ND</v>
       </c>
       <c r="P26" t="str">
         <f t="shared" si="4"/>
-        <v>603-MFR-25FBF52-1K|13</v>
+        <v>603-MFR-25FBF52-1K|15</v>
       </c>
       <c r="Q26" t="str">
         <f t="shared" ref="Q26:Q32" si="7">"Resistor - " &amp; A26&amp;"x "&amp;C26</f>
-        <v>Resistor - 13x 1k</v>
+        <v>Resistor - 15x 1k</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20">
         <f>LEN(B27)-LEN(SUBSTITUTE(B27,",",""))+1</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>200</v>
+        <v>243</v>
       </c>
       <c r="C27" s="14">
         <v>680</v>
@@ -3237,35 +3240,35 @@
         <v>175</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>149</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="L27" s="27">
         <v>0.22</v>
       </c>
       <c r="M27" s="27">
         <f t="shared" si="6"/>
-        <v>1.76</v>
+        <v>0.88</v>
       </c>
       <c r="N27" s="13" t="s">
         <v>108</v>
       </c>
       <c r="O27" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>8,A105963CT-ND</v>
+        <v>4,A105963CT-ND</v>
       </c>
       <c r="P27" t="str">
         <f>IF(NOT(K27=""),K27&amp;"|"&amp;A27,"")</f>
-        <v>279-LR1F680R|8</v>
+        <v>279-LR1F680R|4</v>
       </c>
       <c r="Q27" t="str">
         <f t="shared" si="7"/>
-        <v>Resistor - 8x 680</v>
+        <v>Resistor - 4x 680</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="40" thickBot="1" x14ac:dyDescent="0.25">
@@ -3274,7 +3277,7 @@
         <v>6</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C28" s="3">
         <v>470</v>
@@ -3323,16 +3326,17 @@
     </row>
     <row r="29" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20">
-        <v>2</v>
+        <f>LEN(B29)-LEN(SUBSTITUTE(B29,",",""))+1</f>
+        <v>7</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>134</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -3343,13 +3347,13 @@
         <v>175</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="L29" s="27">
         <v>0.14000000000000001</v>
@@ -3360,15 +3364,15 @@
       <c r="N29" s="6"/>
       <c r="O29" s="4" t="str">
         <f>IF(NOT(J29=""),A29&amp;","&amp;J29,"")</f>
-        <v>2,2.49KXBK-ND</v>
+        <v>7,2.49KXBK-ND</v>
       </c>
       <c r="P29" t="str">
         <f>IF(NOT(K29=""),K29&amp;"|"&amp;A29,"")</f>
-        <v>603-MFR-25FBF52-2K49|2</v>
+        <v>603-MFR-25FBF52-2K49|7</v>
       </c>
       <c r="Q29" t="str">
         <f>"Resistor - " &amp; A29&amp;"x "&amp;C29</f>
-        <v>Resistor - 2x 0.1% 2.49k</v>
+        <v>Resistor - 7x 0.1% 2.49k</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3431,7 +3435,7 @@
         <v>12</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>59</v>
@@ -3448,13 +3452,13 @@
         <v>175</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>62</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="L31" s="27">
         <v>0.1</v>
@@ -3483,7 +3487,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C32" s="3">
         <v>160</v>
@@ -3632,13 +3636,13 @@
         <v>175</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>83</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="L35" s="27">
         <v>15.41</v>
@@ -3666,7 +3670,7 @@
         <v>2</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>137</v>
@@ -4010,7 +4014,7 @@
       </c>
       <c r="M45" s="12">
         <f>SUM(M2:M44)</f>
-        <v>87.28</v>
+        <v>86.36</v>
       </c>
       <c r="N45" s="11" t="s">
         <v>74</v>
@@ -5061,7 +5065,7 @@
         <v>95</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="L23" s="6">
         <v>1.51</v>
@@ -5071,7 +5075,7 @@
         <v>9.06</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="O23" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5298,13 +5302,13 @@
         <v>3</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>134</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>55</v>
@@ -5317,13 +5321,13 @@
         <v>175</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="L29" s="27">
         <v>0.14000000000000001</v>

</xml_diff>